<commit_message>
Se arregla recibos de pago
</commit_message>
<xml_diff>
--- a/datos/nomina_quincenal_pago_20260131.xlsx
+++ b/datos/nomina_quincenal_pago_20260131.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA12"/>
+  <dimension ref="A1:AA14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -573,17 +573,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>171572201</t>
+          <t>3</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Angel Sanguino</t>
+          <t>ANGEL MOLINA</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>CTO</t>
+          <t>AYUDANTE</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -607,7 +607,7 @@
         </is>
       </c>
       <c r="H2" t="n">
-        <v>4.41</v>
+        <v>4.51</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
@@ -625,7 +625,7 @@
         </is>
       </c>
       <c r="L2" t="n">
-        <v>95</v>
+        <v>21</v>
       </c>
       <c r="M2" t="n">
         <v>0</v>
@@ -660,39 +660,35 @@
       <c r="W2" t="n">
         <v>0</v>
       </c>
-      <c r="X2" t="inlineStr">
-        <is>
-          <t>0-465966636460</t>
-        </is>
-      </c>
+      <c r="X2" t="inlineStr"/>
       <c r="Y2" t="inlineStr">
         <is>
-          <t>Banco General</t>
+          <t>BANCO GENERAL</t>
         </is>
       </c>
       <c r="Z2" t="inlineStr">
         <is>
-          <t>Ahorro</t>
+          <t>AHORRO</t>
         </is>
       </c>
       <c r="AA2" t="n">
-        <v>418.95</v>
+        <v>94.70999999999999</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>5-522-224</t>
+          <t>8-879-965</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Carlos Orejuela</t>
+          <t>CARLOS OREJUELA</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Ayudante</t>
+          <t>CABILLERO CALIFICADO</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -716,7 +712,7 @@
         </is>
       </c>
       <c r="H3" t="n">
-        <v>4.41</v>
+        <v>6.1</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
@@ -734,22 +730,22 @@
         </is>
       </c>
       <c r="L3" t="n">
-        <v>33</v>
+        <v>87</v>
       </c>
       <c r="M3" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="N3" t="n">
-        <v>11.03</v>
+        <v>38.12</v>
       </c>
       <c r="O3" t="n">
         <v>0</v>
       </c>
       <c r="P3" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q3" t="n">
-        <v>0</v>
+        <v>73.2</v>
       </c>
       <c r="R3" t="n">
         <v>0</v>
@@ -769,44 +765,40 @@
       <c r="W3" t="n">
         <v>0</v>
       </c>
-      <c r="X3" t="inlineStr">
-        <is>
-          <t>0-472979646813</t>
-        </is>
-      </c>
+      <c r="X3" t="inlineStr"/>
       <c r="Y3" t="inlineStr">
         <is>
-          <t>Banco General</t>
+          <t>BANCO GENERAL</t>
         </is>
       </c>
       <c r="Z3" t="inlineStr">
         <is>
-          <t>Ahorro</t>
+          <t>AHORROS</t>
         </is>
       </c>
       <c r="AA3" t="n">
-        <v>147.74</v>
+        <v>562.72</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>9-706-1114</t>
+          <t>8-970-1644</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Edionel Rodriguez</t>
+          <t>DEBIN GONZALES</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Empleado calificado</t>
+          <t>AYUDANTE</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Empleado Fijo</t>
+          <t>Por horas</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -816,7 +808,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Sí</t>
+          <t>No</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -825,7 +817,7 @@
         </is>
       </c>
       <c r="H4" t="n">
-        <v>5.98</v>
+        <v>4.51</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
@@ -843,22 +835,22 @@
         </is>
       </c>
       <c r="L4" t="n">
-        <v>131</v>
+        <v>77</v>
       </c>
       <c r="M4" t="n">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="N4" t="n">
-        <v>209.3</v>
+        <v>16.91</v>
       </c>
       <c r="O4" t="n">
-        <v>115.94</v>
+        <v>0</v>
       </c>
       <c r="P4" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q4" t="n">
-        <v>0</v>
+        <v>54.12</v>
       </c>
       <c r="R4" t="n">
         <v>0</v>
@@ -878,39 +870,35 @@
       <c r="W4" t="n">
         <v>0</v>
       </c>
-      <c r="X4" t="inlineStr">
-        <is>
-          <t>0-465972284592</t>
-        </is>
-      </c>
+      <c r="X4" t="inlineStr"/>
       <c r="Y4" t="inlineStr">
         <is>
-          <t>Banco General</t>
+          <t>BANCO GENERAL</t>
         </is>
       </c>
       <c r="Z4" t="inlineStr">
         <is>
-          <t>Ahorro</t>
+          <t>AHORROS</t>
         </is>
       </c>
       <c r="AA4" t="n">
-        <v>825.24</v>
+        <v>368.69</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>8-098-2345</t>
+          <t>8-863-1584</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Eliseo Montilla</t>
+          <t>EDWIN FIGUEROA</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Ayudante</t>
+          <t>AYUDANTE</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -934,7 +922,7 @@
         </is>
       </c>
       <c r="H5" t="n">
-        <v>4.41</v>
+        <v>4.51</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
@@ -952,22 +940,22 @@
         </is>
       </c>
       <c r="L5" t="n">
+        <v>79</v>
+      </c>
+      <c r="M5" t="n">
+        <v>5</v>
+      </c>
+      <c r="N5" t="n">
+        <v>28.19</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" t="n">
         <v>8</v>
       </c>
-      <c r="M5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N5" t="n">
-        <v>0</v>
-      </c>
-      <c r="O5" t="n">
-        <v>0</v>
-      </c>
-      <c r="P5" t="n">
-        <v>0</v>
-      </c>
       <c r="Q5" t="n">
-        <v>0</v>
+        <v>54.12</v>
       </c>
       <c r="R5" t="n">
         <v>0</v>
@@ -990,37 +978,37 @@
       <c r="X5" t="inlineStr"/>
       <c r="Y5" t="inlineStr">
         <is>
-          <t>Banco General</t>
+          <t>BANCO GENERAL</t>
         </is>
       </c>
       <c r="Z5" t="inlineStr">
         <is>
-          <t>Ahorro</t>
+          <t>AHORROS</t>
         </is>
       </c>
       <c r="AA5" t="n">
-        <v>35.28</v>
+        <v>379.97</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>8-847-2279</t>
+          <t>8-921-1193</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Eulises Camaño</t>
+          <t>EDWIN VEGA</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Soldador</t>
+          <t>AYUDANTE</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Empleado Fijo</t>
+          <t>Por horas</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -1030,7 +1018,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Sí</t>
+          <t>No</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -1039,7 +1027,7 @@
         </is>
       </c>
       <c r="H6" t="n">
-        <v>5.98</v>
+        <v>4.51</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
@@ -1057,22 +1045,22 @@
         </is>
       </c>
       <c r="L6" t="n">
-        <v>112</v>
+        <v>77</v>
       </c>
       <c r="M6" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="N6" t="n">
-        <v>67.28</v>
+        <v>16.91</v>
       </c>
       <c r="O6" t="n">
-        <v>115.94</v>
+        <v>0</v>
       </c>
       <c r="P6" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q6" t="n">
-        <v>0</v>
+        <v>54.12</v>
       </c>
       <c r="R6" t="n">
         <v>0</v>
@@ -1092,39 +1080,35 @@
       <c r="W6" t="n">
         <v>0</v>
       </c>
-      <c r="X6" t="inlineStr">
-        <is>
-          <t>0-441988638943</t>
-        </is>
-      </c>
+      <c r="X6" t="inlineStr"/>
       <c r="Y6" t="inlineStr">
         <is>
-          <t>Banco General</t>
+          <t>BANCO GENERAL</t>
         </is>
       </c>
       <c r="Z6" t="inlineStr">
         <is>
-          <t>Ahorro</t>
+          <t>AHORROS</t>
         </is>
       </c>
       <c r="AA6" t="n">
-        <v>683.22</v>
+        <v>368.69</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>8-579-7976</t>
+          <t>1-716-753</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Ezequiel Montilla</t>
+          <t>ESTEBAN PALACIO</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Topografo</t>
+          <t>AYUDANTE</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1148,7 +1132,7 @@
         </is>
       </c>
       <c r="H7" t="n">
-        <v>4.41</v>
+        <v>4.51</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
@@ -1166,22 +1150,22 @@
         </is>
       </c>
       <c r="L7" t="n">
-        <v>3.5</v>
+        <v>84</v>
       </c>
       <c r="M7" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="N7" t="n">
-        <v>0</v>
+        <v>56.37</v>
       </c>
       <c r="O7" t="n">
         <v>0</v>
       </c>
       <c r="P7" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q7" t="n">
-        <v>0</v>
+        <v>54.12</v>
       </c>
       <c r="R7" t="n">
         <v>0</v>
@@ -1204,16 +1188,16 @@
       <c r="X7" t="inlineStr"/>
       <c r="Y7" t="inlineStr">
         <is>
-          <t>Banco General</t>
+          <t>BANCO GENERAL</t>
         </is>
       </c>
       <c r="Z7" t="inlineStr">
         <is>
-          <t>Ahorro</t>
+          <t>AHORROS</t>
         </is>
       </c>
       <c r="AA7" t="n">
-        <v>15.44</v>
+        <v>408.15</v>
       </c>
     </row>
     <row r="8">
@@ -1224,12 +1208,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Jaime Martinez</t>
+          <t>JAIME MARTINEZ</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Ayudante</t>
+          <t>AYUDANTE</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -1253,7 +1237,7 @@
         </is>
       </c>
       <c r="H8" t="n">
-        <v>4.41</v>
+        <v>4.51</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
@@ -1271,7 +1255,7 @@
         </is>
       </c>
       <c r="L8" t="n">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="M8" t="n">
         <v>0</v>
@@ -1313,32 +1297,32 @@
       </c>
       <c r="Y8" t="inlineStr">
         <is>
-          <t>Banco General</t>
+          <t>BANCO GENERAL</t>
         </is>
       </c>
       <c r="Z8" t="inlineStr">
         <is>
-          <t>Ahorro</t>
+          <t>AHORRO</t>
         </is>
       </c>
       <c r="AA8" t="n">
-        <v>35.28</v>
+        <v>130.79</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>6-718-1627</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>José Rodriguez</t>
+          <t>JOSE BENITO CHIRINOS</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Ayudante</t>
+          <t>AYUDANTE</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -1362,7 +1346,7 @@
         </is>
       </c>
       <c r="H9" t="n">
-        <v>4.41</v>
+        <v>4.51</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
@@ -1380,22 +1364,22 @@
         </is>
       </c>
       <c r="L9" t="n">
-        <v>128.33</v>
+        <v>45</v>
       </c>
       <c r="M9" t="n">
-        <v>19.83</v>
+        <v>0</v>
       </c>
       <c r="N9" t="n">
-        <v>109.33</v>
+        <v>0</v>
       </c>
       <c r="O9" t="n">
         <v>0</v>
       </c>
       <c r="P9" t="n">
-        <v>5.5</v>
+        <v>0</v>
       </c>
       <c r="Q9" t="n">
-        <v>36.38</v>
+        <v>0</v>
       </c>
       <c r="R9" t="n">
         <v>0</v>
@@ -1415,44 +1399,36 @@
       <c r="W9" t="n">
         <v>0</v>
       </c>
-      <c r="X9" t="inlineStr">
-        <is>
-          <t>0-419972553348</t>
-        </is>
-      </c>
+      <c r="X9" t="inlineStr"/>
       <c r="Y9" t="inlineStr">
         <is>
-          <t>Banco General</t>
-        </is>
-      </c>
-      <c r="Z9" t="inlineStr">
-        <is>
-          <t>Ahorro</t>
-        </is>
-      </c>
+          <t>BANCO GENERAL</t>
+        </is>
+      </c>
+      <c r="Z9" t="inlineStr"/>
       <c r="AA9" t="n">
-        <v>599.9400000000001</v>
+        <v>202.95</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>5-704-561</t>
+          <t>8-771-179</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Misael Cedeño</t>
+          <t>JUAN RENTERIA</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Soldador</t>
+          <t>ALBAÑIL CALIFICADO</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Empleado Fijo</t>
+          <t>Por horas</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -1462,7 +1438,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Sí</t>
+          <t>No</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -1471,7 +1447,7 @@
         </is>
       </c>
       <c r="H10" t="n">
-        <v>5.98</v>
+        <v>6.1</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
@@ -1489,22 +1465,22 @@
         </is>
       </c>
       <c r="L10" t="n">
-        <v>102</v>
+        <v>62</v>
       </c>
       <c r="M10" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N10" t="n">
-        <v>0</v>
+        <v>30.5</v>
       </c>
       <c r="O10" t="n">
-        <v>109.96</v>
+        <v>0</v>
       </c>
       <c r="P10" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q10" t="n">
-        <v>0</v>
+        <v>73.2</v>
       </c>
       <c r="R10" t="n">
         <v>0</v>
@@ -1524,39 +1500,35 @@
       <c r="W10" t="n">
         <v>0</v>
       </c>
-      <c r="X10" t="inlineStr">
-        <is>
-          <t>0-465960167120</t>
-        </is>
-      </c>
+      <c r="X10" t="inlineStr"/>
       <c r="Y10" t="inlineStr">
         <is>
-          <t>Banco General</t>
+          <t>BANCO GENERAL</t>
         </is>
       </c>
       <c r="Z10" t="inlineStr">
         <is>
-          <t>Ahorro</t>
+          <t>AHORROS</t>
         </is>
       </c>
       <c r="AA10" t="n">
-        <v>609.96</v>
+        <v>408.7</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>8-1042-173</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Pedro Cuevas</t>
+          <t>LUIS FRIAS</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Ayudante</t>
+          <t>AYUDANTE</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1580,7 +1552,7 @@
         </is>
       </c>
       <c r="H11" t="n">
-        <v>4.41</v>
+        <v>4.51</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
@@ -1598,22 +1570,22 @@
         </is>
       </c>
       <c r="L11" t="n">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="M11" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N11" t="n">
-        <v>0</v>
+        <v>16.91</v>
       </c>
       <c r="O11" t="n">
         <v>0</v>
       </c>
       <c r="P11" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q11" t="n">
-        <v>0</v>
+        <v>54.12</v>
       </c>
       <c r="R11" t="n">
         <v>0</v>
@@ -1633,39 +1605,35 @@
       <c r="W11" t="n">
         <v>0</v>
       </c>
-      <c r="X11" t="inlineStr">
-        <is>
-          <t>0-472963882991</t>
-        </is>
-      </c>
+      <c r="X11" t="inlineStr"/>
       <c r="Y11" t="inlineStr">
         <is>
-          <t>Banco General</t>
+          <t>BANCO GENERAL</t>
         </is>
       </c>
       <c r="Z11" t="inlineStr">
         <is>
-          <t>Ahorro</t>
+          <t>AHORRO</t>
         </is>
       </c>
       <c r="AA11" t="n">
-        <v>163.17</v>
+        <v>89.06999999999999</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>160423173</t>
+          <t>8-730-847</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Ramón Rodriguez</t>
+          <t>ORNELIS BARRIOS</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Carpintero</t>
+          <t>ALBAÑIL PRINPIPIANTE</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -1689,76 +1657,286 @@
         </is>
       </c>
       <c r="H12" t="n">
+        <v>5.09</v>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>16/01/2026</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>30/01/2026</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>31/01/2026</t>
+        </is>
+      </c>
+      <c r="L12" t="n">
+        <v>69</v>
+      </c>
+      <c r="M12" t="n">
+        <v>3</v>
+      </c>
+      <c r="N12" t="n">
+        <v>19.09</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0</v>
+      </c>
+      <c r="P12" t="n">
+        <v>8</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>61.08</v>
+      </c>
+      <c r="R12" t="n">
+        <v>0</v>
+      </c>
+      <c r="S12" t="n">
+        <v>0</v>
+      </c>
+      <c r="T12" t="n">
+        <v>0</v>
+      </c>
+      <c r="U12" t="n">
+        <v>0</v>
+      </c>
+      <c r="V12" t="n">
+        <v>0</v>
+      </c>
+      <c r="W12" t="n">
+        <v>0</v>
+      </c>
+      <c r="X12" t="inlineStr"/>
+      <c r="Y12" t="inlineStr">
+        <is>
+          <t>BANCO GENERAL</t>
+        </is>
+      </c>
+      <c r="Z12" t="inlineStr">
+        <is>
+          <t>AHORROS</t>
+        </is>
+      </c>
+      <c r="AA12" t="n">
+        <v>375.39</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>8-1042-173</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>PEDRO CUEVAS</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>AYUDANTE</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Por horas</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H13" t="n">
+        <v>4.51</v>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>16/01/2026</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>30/01/2026</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>31/01/2026</t>
+        </is>
+      </c>
+      <c r="L13" t="n">
+        <v>37</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0</v>
+      </c>
+      <c r="N13" t="n">
+        <v>0</v>
+      </c>
+      <c r="O13" t="n">
+        <v>0</v>
+      </c>
+      <c r="P13" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>0</v>
+      </c>
+      <c r="R13" t="n">
+        <v>0</v>
+      </c>
+      <c r="S13" t="n">
+        <v>0</v>
+      </c>
+      <c r="T13" t="n">
+        <v>0</v>
+      </c>
+      <c r="U13" t="n">
+        <v>0</v>
+      </c>
+      <c r="V13" t="n">
+        <v>0</v>
+      </c>
+      <c r="W13" t="n">
+        <v>0</v>
+      </c>
+      <c r="X13" t="inlineStr">
+        <is>
+          <t>0-472963882991</t>
+        </is>
+      </c>
+      <c r="Y13" t="inlineStr">
+        <is>
+          <t>BANCO GENERAL</t>
+        </is>
+      </c>
+      <c r="Z13" t="inlineStr">
+        <is>
+          <t>AHORRO</t>
+        </is>
+      </c>
+      <c r="AA13" t="n">
+        <v>166.87</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>8-944-1234</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>XAVIER SAENZ</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>CABILLERO CALIFICADO</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Por horas</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H14" t="n">
+        <v>6.1</v>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>16/01/2026</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>30/01/2026</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>31/01/2026</t>
+        </is>
+      </c>
+      <c r="L14" t="n">
+        <v>79</v>
+      </c>
+      <c r="M14" t="n">
         <v>5</v>
       </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>16/01/2026</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>30/01/2026</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>31/01/2026</t>
-        </is>
-      </c>
-      <c r="L12" t="n">
-        <v>37</v>
-      </c>
-      <c r="M12" t="n">
-        <v>0</v>
-      </c>
-      <c r="N12" t="n">
-        <v>0</v>
-      </c>
-      <c r="O12" t="n">
-        <v>0</v>
-      </c>
-      <c r="P12" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q12" t="n">
-        <v>0</v>
-      </c>
-      <c r="R12" t="n">
-        <v>0</v>
-      </c>
-      <c r="S12" t="n">
-        <v>0</v>
-      </c>
-      <c r="T12" t="n">
-        <v>0</v>
-      </c>
-      <c r="U12" t="n">
-        <v>0</v>
-      </c>
-      <c r="V12" t="n">
-        <v>0</v>
-      </c>
-      <c r="W12" t="n">
-        <v>0</v>
-      </c>
-      <c r="X12" t="inlineStr">
-        <is>
-          <t>0-465984269473</t>
-        </is>
-      </c>
-      <c r="Y12" t="inlineStr">
-        <is>
-          <t>Banco General</t>
-        </is>
-      </c>
-      <c r="Z12" t="inlineStr">
-        <is>
-          <t>Ahorro</t>
-        </is>
-      </c>
-      <c r="AA12" t="n">
-        <v>185</v>
+      <c r="N14" t="n">
+        <v>38.12</v>
+      </c>
+      <c r="O14" t="n">
+        <v>0</v>
+      </c>
+      <c r="P14" t="n">
+        <v>8</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>73.2</v>
+      </c>
+      <c r="R14" t="n">
+        <v>0</v>
+      </c>
+      <c r="S14" t="n">
+        <v>0</v>
+      </c>
+      <c r="T14" t="n">
+        <v>0</v>
+      </c>
+      <c r="U14" t="n">
+        <v>0</v>
+      </c>
+      <c r="V14" t="n">
+        <v>0</v>
+      </c>
+      <c r="W14" t="n">
+        <v>0</v>
+      </c>
+      <c r="X14" t="inlineStr"/>
+      <c r="Y14" t="inlineStr">
+        <is>
+          <t>BANCO GENERAL</t>
+        </is>
+      </c>
+      <c r="Z14" t="inlineStr">
+        <is>
+          <t>AHORROS</t>
+        </is>
+      </c>
+      <c r="AA14" t="n">
+        <v>513.92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>